<commit_message>
Revert "Removed gate transistors"
</commit_message>
<xml_diff>
--- a/source/JLCPCB and LCSC/JLCPCB BOM Cheap FOCer 2 v1.0.xlsx
+++ b/source/JLCPCB and LCSC/JLCPCB BOM Cheap FOCer 2 v1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Projects/kicad/Cheap-FOCer-2/source/JLCPCB and LCSC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Desktop\KiCAD Projects\Cheap FOCer 2 60mm\design\JLCPCB and LCSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F013ACB8-E9CF-7D4E-9317-A81D2717C677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6AFE1F-80EC-4A3E-B5C5-A0A178BD5181}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="2840" windowWidth="27020" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="210">
   <si>
     <t>Footprint</t>
   </si>
@@ -567,6 +567,12 @@
     <t>R13, R14, R22, R23, R34, R35, R64, R65</t>
   </si>
   <si>
+    <t>R75, R76, R77, R78, R79, R80</t>
+  </si>
+  <si>
+    <t>4.7R</t>
+  </si>
+  <si>
     <t>R24, R66, R67, R69, R70</t>
   </si>
   <si>
@@ -600,6 +606,15 @@
     <t>D_SOD-323</t>
   </si>
   <si>
+    <t>Q7, Q8, Q9, Q10, Q11, Q12</t>
+  </si>
+  <si>
+    <t>Q_PNP_BCE</t>
+  </si>
+  <si>
+    <t>SOT-23</t>
+  </si>
+  <si>
     <t>JST_PH_B3B-PH-K_1x03_P2.00mm_Vertical_hybrid</t>
   </si>
   <si>
@@ -616,6 +631,12 @@
   </si>
   <si>
     <t>C78395</t>
+  </si>
+  <si>
+    <t>C8542</t>
+  </si>
+  <si>
+    <t>C23164</t>
   </si>
   <si>
     <t>C22843</t>
@@ -754,8 +775,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1033,24 +1054,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.83203125" customWidth="1"/>
-    <col min="8" max="8" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.77734375" customWidth="1"/>
+    <col min="8" max="8" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -1067,7 +1088,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="26.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>115</v>
       </c>
@@ -1087,7 +1108,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -1104,7 +1125,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1121,7 +1142,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1138,7 +1159,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -1155,7 +1176,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>175</v>
       </c>
@@ -1166,13 +1187,13 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="E7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1189,7 +1210,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1206,7 +1227,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -1223,7 +1244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>117</v>
       </c>
@@ -1240,7 +1261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -1257,7 +1278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -1274,7 +1295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>101</v>
       </c>
@@ -1291,7 +1312,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -1308,7 +1329,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>59</v>
       </c>
@@ -1325,7 +1346,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>61</v>
       </c>
@@ -1342,7 +1363,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -1359,7 +1380,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1376,7 +1397,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -1393,7 +1414,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1410,9 +1431,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
       <c r="B22" t="s">
         <v>180</v>
@@ -1421,632 +1442,666 @@
         <v>8</v>
       </c>
       <c r="D22" t="s">
-        <v>132</v>
+        <v>203</v>
       </c>
       <c r="E22">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>182</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E23">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>182</v>
+        <v>65</v>
       </c>
       <c r="B24" t="s">
-        <v>181</v>
+        <v>64</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
       </c>
       <c r="D24" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="E24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>183</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>137</v>
+        <v>204</v>
       </c>
       <c r="E25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>194</v>
+        <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E26">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>68</v>
+        <v>199</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="C27" t="s">
         <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B28" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="C28" t="s">
         <v>8</v>
       </c>
       <c r="D28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E28">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>69</v>
       </c>
       <c r="C29" t="s">
         <v>8</v>
       </c>
       <c r="D29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E29">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B30" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="C30" t="s">
         <v>8</v>
       </c>
       <c r="D30" t="s">
+        <v>141</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" t="s">
         <v>142</v>
       </c>
-      <c r="E30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>74</v>
-      </c>
-      <c r="B31" t="s">
-        <v>183</v>
-      </c>
-      <c r="C31" t="s">
-        <v>75</v>
-      </c>
-      <c r="D31" t="s">
-        <v>143</v>
-      </c>
       <c r="E31">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>74</v>
       </c>
       <c r="B32" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C32" t="s">
         <v>75</v>
       </c>
       <c r="D32" t="s">
-        <v>195</v>
+        <v>143</v>
       </c>
       <c r="E32">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>77</v>
+        <v>181</v>
       </c>
       <c r="B33" t="s">
-        <v>76</v>
+        <v>186</v>
       </c>
       <c r="C33" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D33" t="s">
-        <v>144</v>
+        <v>200</v>
       </c>
       <c r="E33">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" t="s">
+        <v>144</v>
+      </c>
+      <c r="E34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>17</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>81</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>103</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>145</v>
       </c>
-      <c r="E35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>186</v>
-      </c>
-      <c r="B36" t="s">
-        <v>185</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="E36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>188</v>
+      </c>
+      <c r="B37" t="s">
         <v>187</v>
       </c>
-      <c r="D36" t="s">
-        <v>196</v>
-      </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="C37" t="s">
         <v>189</v>
       </c>
-      <c r="B37" t="s">
-        <v>188</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
+        <v>201</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>191</v>
+      </c>
+      <c r="B38" t="s">
         <v>190</v>
       </c>
-      <c r="D37" t="s">
+      <c r="C38" t="s">
         <v>192</v>
       </c>
-      <c r="E37">
+      <c r="D38" t="s">
+        <v>197</v>
+      </c>
+      <c r="E38">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>104</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>92</v>
-      </c>
-      <c r="C38" t="s">
-        <v>18</v>
-      </c>
-      <c r="D38" t="s">
-        <v>146</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>105</v>
-      </c>
-      <c r="B39" t="s">
-        <v>19</v>
       </c>
       <c r="C39" t="s">
         <v>18</v>
       </c>
       <c r="D39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E39">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C40" t="s">
         <v>18</v>
       </c>
       <c r="D40" t="s">
+        <v>147</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" t="s">
         <v>148</v>
       </c>
-      <c r="E40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="E41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>83</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>82</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>21</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>149</v>
       </c>
-      <c r="E41">
+      <c r="E42">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="E42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
+      <c r="E43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="E43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="D44" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>110</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>23</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>24</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>150</v>
       </c>
-      <c r="E44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="E45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>111</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>25</v>
-      </c>
-      <c r="C45" t="s">
-        <v>26</v>
-      </c>
-      <c r="D45" t="s">
-        <v>151</v>
-      </c>
-      <c r="E45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>112</v>
-      </c>
-      <c r="B46" t="s">
-        <v>27</v>
       </c>
       <c r="C46" t="s">
         <v>26</v>
       </c>
       <c r="D46" t="s">
+        <v>151</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>112</v>
+      </c>
+      <c r="B47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" t="s">
         <v>152</v>
       </c>
-      <c r="E46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="E47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>113</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>28</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>29</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D48" t="s">
         <v>153</v>
       </c>
-      <c r="E47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="E48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>114</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>86</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>30</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>154</v>
       </c>
-      <c r="E48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="E49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>37</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>36</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>8</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>155</v>
       </c>
-      <c r="E49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
+      <c r="E50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>194</v>
+      </c>
+      <c r="B51" t="s">
+        <v>193</v>
+      </c>
+      <c r="C51" t="s">
+        <v>195</v>
+      </c>
+      <c r="D51" t="s">
+        <v>202</v>
+      </c>
+      <c r="E51">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D52" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E50">
+      <c r="E52">
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D53" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="E51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
+      <c r="E53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C54" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
+      <c r="D54" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B55" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C55" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
+      <c r="D55" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="E54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
+      <c r="C56" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="E55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
+      <c r="D57" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D58" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="E56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
+      <c r="E58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C59" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="E57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
+      <c r="D59" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B60" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E58">
+      <c r="E60">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D52" r:id="rId1" display="https://lcsc.com/product-detail/Wire-To-Board-Wire-To-Wire-Connector_BOOMELE-Boom-Precision-Elec-PH-2A_C2319.html" xr:uid="{BE2B1760-F370-460C-86A3-BA43A038EA6A}"/>
-    <hyperlink ref="D53" r:id="rId2" display="https://lcsc.com/product-detail/Wire-To-Board-Wire-To-Wire-Connector_BOOMELE-Boom-Precision-Elec-PH-2A_C2319.html" xr:uid="{CC73C431-FC33-4779-85FE-4E4F3EE78FDE}"/>
-    <hyperlink ref="D54" r:id="rId3" display="https://lcsc.com/product-detail/Wire-To-Board-Wire-To-Wire-Connector_BOOMELE-Boom-Precision-Elec-PH-3A_C2320.html" xr:uid="{D5ACCC8C-1F1B-47B7-9C9F-B6FAD2800E9D}"/>
-    <hyperlink ref="D55" r:id="rId4" display="https://lcsc.com/product-detail/Wire-To-Board-Wire-To-Wire-Connector_BOOMELE-Boom-Precision-Elec-PH-7A_C10398.html" xr:uid="{A2A064D5-7799-46C6-8F83-8B744BCE7B4B}"/>
-    <hyperlink ref="D57" r:id="rId5" display="https://lcsc.com/product-detail/Wire-To-Board-Wire-To-Wire-Connector_BOOMELE-Boom-Precision-Elec-PH-6A_C33478.html" xr:uid="{358B7910-EFCE-4A84-B386-C8E2B0006ED5}"/>
+    <hyperlink ref="D54" r:id="rId1" display="https://lcsc.com/product-detail/Wire-To-Board-Wire-To-Wire-Connector_BOOMELE-Boom-Precision-Elec-PH-2A_C2319.html" xr:uid="{BE2B1760-F370-460C-86A3-BA43A038EA6A}"/>
+    <hyperlink ref="D55" r:id="rId2" display="https://lcsc.com/product-detail/Wire-To-Board-Wire-To-Wire-Connector_BOOMELE-Boom-Precision-Elec-PH-2A_C2319.html" xr:uid="{CC73C431-FC33-4779-85FE-4E4F3EE78FDE}"/>
+    <hyperlink ref="D56" r:id="rId3" display="https://lcsc.com/product-detail/Wire-To-Board-Wire-To-Wire-Connector_BOOMELE-Boom-Precision-Elec-PH-3A_C2320.html" xr:uid="{D5ACCC8C-1F1B-47B7-9C9F-B6FAD2800E9D}"/>
+    <hyperlink ref="D57" r:id="rId4" display="https://lcsc.com/product-detail/Wire-To-Board-Wire-To-Wire-Connector_BOOMELE-Boom-Precision-Elec-PH-7A_C10398.html" xr:uid="{A2A064D5-7799-46C6-8F83-8B744BCE7B4B}"/>
+    <hyperlink ref="D59" r:id="rId5" display="https://lcsc.com/product-detail/Wire-To-Board-Wire-To-Wire-Connector_BOOMELE-Boom-Precision-Elec-PH-6A_C33478.html" xr:uid="{358B7910-EFCE-4A84-B386-C8E2B0006ED5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>